<commit_message>
identification workflow avec condition + champ done
</commit_message>
<xml_diff>
--- a/src/main/Configuration/RulesTest.xlsx
+++ b/src/main/Configuration/RulesTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Workflow name</t>
   </si>
@@ -32,15 +32,6 @@
     <t>Condition</t>
   </si>
   <si>
-    <t>CHAMP_DEMANDE_TYPE</t>
-  </si>
-  <si>
-    <t>REGLE_DEMANDE_TYPE</t>
-  </si>
-  <si>
-    <t>CHAMP_Type_TITRE</t>
-  </si>
-  <si>
     <t>REGLE_TYPE_TITRE</t>
   </si>
   <si>
@@ -77,35 +68,38 @@
     <t>Demande passeport adulte</t>
   </si>
   <si>
-    <t>value!=null</t>
-  </si>
-  <si>
-    <t>value!=null &amp;&amp; age &lt;18</t>
-  </si>
-  <si>
-    <t>DEMANDE_TYPE==DEMANDE &amp;&amp; age &lt;18</t>
-  </si>
-  <si>
-    <t>value=="PSP"</t>
-  </si>
-  <si>
-    <t>value=="CNIE"</t>
-  </si>
-  <si>
-    <t>DEMANDE_TYPE==DEMANDE &amp;&amp; age&lt;18</t>
-  </si>
-  <si>
-    <t>DEMANDE_TYPE==DEMANDE &amp;&amp; age &gt;= 18</t>
-  </si>
-  <si>
-    <t>value!=null &amp;&amp; age &gt;= 18</t>
+    <t>%value%!=null</t>
+  </si>
+  <si>
+    <t>%value%=="PSP"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Minor_Check(%CHAMP_DATE_NAISSANCE%, 18)</t>
+  </si>
+  <si>
+    <t>Minor_Check(%CHAMP_DATE_NAISSANCE%, 18)</t>
+  </si>
+  <si>
+    <t>!Minor_Check(%CHAMP_DATE_NAISSANCE%, 18)</t>
+  </si>
+  <si>
+    <t>CHAMP_TYPE_TITRE</t>
+  </si>
+  <si>
+    <t>%value%=="CNIE"</t>
+  </si>
+  <si>
+    <t>%value% !=null &amp;&amp;  Minor_Check(%value%,18)</t>
+  </si>
+  <si>
+    <t>%value% !=null &amp;&amp; Minor_Check(%value%,18)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +125,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -253,7 +254,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -279,6 +279,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,170 +562,156 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.109375" customWidth="1"/>
-    <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="66.88671875" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
     <col min="6" max="6" width="20.21875" customWidth="1"/>
     <col min="7" max="7" width="23.88671875" customWidth="1"/>
     <col min="8" max="8" width="23.77734375" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" customWidth="1"/>
     <col min="11" max="11" width="17.33203125" customWidth="1"/>
     <col min="12" max="12" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="L2" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="3" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="14"/>
+      <c r="K4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="15" t="s">
         <v>14</v>
-      </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout loadData pour json et mise ajour sctruture code
</commit_message>
<xml_diff>
--- a/src/main/Configuration/RulesTest.xlsx
+++ b/src/main/Configuration/RulesTest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="77">
   <si>
     <t xml:space="preserve">Workflow name</t>
   </si>
@@ -188,36 +188,12 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">value!= null &amp;&amp; BelongTo(value, “mineur</t>
+      <t xml:space="preserve">NotNull(value)&amp;&amp; BelongTo(value, </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MINEUR,Mineur”)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">NotNull(value) &amp;&amp; BelongTo(value,"F,H,femme,homme,Femme,Homme,FEMME,HOMME")</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -225,7 +201,17 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">(NotNull(value) &amp;&amp; Length_Between</t>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">mineur,MINEUR,Mineur</t>
     </r>
     <r>
       <rPr>
@@ -233,10 +219,25 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(value,1,76) &amp;&amp; IsValidName(value)) || IsNull(value)</t>
+      <t xml:space="preserve">)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NotNull(value) &amp;&amp; BelongTo(value,"F,H,femme,homme,Femme,Homme,FEMME,HOMME")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NotNull(value) &amp;&amp; Length_Between(value,1,76) &amp;&amp; IsValidName(value)) || IsNull(value)</t>
   </si>
   <si>
     <t xml:space="preserve">NotNull(value) &amp;&amp; Length_Between(value,1,15) &amp;&amp; IsValidName(value)</t>
@@ -289,54 +290,7 @@
     <t xml:space="preserve">value=="CNIE"</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">value!= null &amp;&amp; BelongTo(value, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">mineur,MINEUR,Mineur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">NotNull(value)&amp;&amp; BelongTo(value, "mineur,MINEUR,Mineur")</t>
   </si>
   <si>
     <t xml:space="preserve">Première Demande passeport adulte</t>
@@ -348,54 +302,7 @@
     <t xml:space="preserve">NotNull(value) &amp;&amp; Major_Check(value)  &amp;&amp; Valid_Date(value)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">value!= null &amp;&amp; BelongTo(value,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">majeur,MAJEUR,Majeur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">NotNull(value)&amp;&amp; BelongTo(value,"majeur,MAJEUR,Majeur")</t>
   </si>
   <si>
     <t xml:space="preserve">NO</t>
@@ -411,53 +318,6 @@
   </si>
   <si>
     <t xml:space="preserve">NotNull(value)   &amp;&amp;  Minor_Check(value) &amp;&amp; Valid_Date(value)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">value!= null &amp;&amp; BelongTo(value, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">mineur,MINEUR,Mineur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -467,7 +327,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,19 +367,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -537,12 +384,6 @@
       <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -667,7 +508,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -676,10 +517,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -712,15 +549,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -728,7 +561,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -740,15 +573,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1003,11 +832,11 @@
   </sheetPr>
   <dimension ref="A1:AU6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AO1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AQ2" activeCellId="0" sqref="AQ2:AQ6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P4" activeCellId="0" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="47.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.22"/>
@@ -1048,851 +877,851 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="22.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="74.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="32.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="48" style="2" width="8.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="48" style="1" width="8.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AH1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AM1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AN1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="6" t="s">
+      <c r="AO1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AP1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="AR1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="6" t="s">
+      <c r="AS1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="6" t="s">
+      <c r="AT1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AU1" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" s="14" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+    <row r="2" s="12" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="E2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="9" t="s">
+      <c r="K2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2" s="11" t="s">
+      <c r="N2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="10" t="s">
+      <c r="Q2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="T2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="12" t="s">
+      <c r="T2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="W2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y2" s="10" t="s">
+      <c r="W2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Z2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB2" s="10" t="s">
+      <c r="Z2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AC2" s="10" t="s">
+      <c r="AC2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AD2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE2" s="10" t="s">
+      <c r="AD2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AF2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH2" s="10" t="s">
+      <c r="AF2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AI2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AK2" s="10" t="s">
+      <c r="AI2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AL2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AN2" s="10" t="s">
+      <c r="AL2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AO2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ2" s="13" t="s">
+      <c r="AO2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AR2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AT2" s="10" t="s">
+      <c r="AR2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AU2" s="10" t="s">
+      <c r="AU2" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" s="14" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+    <row r="3" s="12" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="E3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="9" t="s">
+      <c r="K3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="P3" s="11" t="s">
+      <c r="N3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="Q3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="S3" s="10" t="s">
+      <c r="Q3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="S3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="V3" s="12" t="s">
+      <c r="T3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="V3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="W3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="X3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y3" s="10" t="s">
+      <c r="W3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="X3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Z3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB3" s="10" t="s">
+      <c r="Z3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AC3" s="10" t="s">
+      <c r="AC3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AD3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE3" s="10" t="s">
+      <c r="AD3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AF3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH3" s="10" t="s">
+      <c r="AF3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AI3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AK3" s="10" t="s">
+      <c r="AI3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AL3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AN3" s="10" t="s">
+      <c r="AL3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AO3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ3" s="13" t="s">
+      <c r="AO3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AR3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AT3" s="10" t="s">
+      <c r="AR3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AU3" s="10" t="s">
+      <c r="AU3" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" s="14" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+    <row r="4" s="12" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="17" t="s">
+      <c r="C4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="17" t="s">
+      <c r="E4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="M4" s="9" t="s">
+      <c r="K4" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="N4" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="11" t="s">
+      <c r="N4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="P4" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="Q4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="S4" s="10" t="s">
+      <c r="Q4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="S4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="T4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="U4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="V4" s="12" t="s">
+      <c r="T4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="V4" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="W4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="X4" s="10" t="s">
+      <c r="W4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="X4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Y4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Z4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB4" s="10" t="s">
+      <c r="Z4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AC4" s="10" t="s">
+      <c r="AC4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AD4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE4" s="10" t="s">
+      <c r="AD4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AF4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH4" s="10" t="s">
+      <c r="AF4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AI4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AK4" s="10" t="s">
+      <c r="AI4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AL4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AN4" s="10" t="s">
+      <c r="AL4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AO4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ4" s="13" t="s">
+      <c r="AO4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ4" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AR4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS4" s="10" t="s">
+      <c r="AR4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="AT4" s="10"/>
+      <c r="AT4" s="9"/>
     </row>
-    <row r="5" s="14" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+    <row r="5" s="12" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="17" t="s">
+      <c r="C5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="17" t="s">
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="8" t="s">
+      <c r="I5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M5" s="9" t="s">
+      <c r="K5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="N5" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="P5" s="11" t="s">
+      <c r="N5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="Q5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="S5" s="10" t="s">
+      <c r="Q5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="T5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="U5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="V5" s="12" t="s">
+      <c r="T5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="V5" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="W5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="X5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y5" s="10" t="s">
+      <c r="W5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y5" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Z5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB5" s="10" t="s">
+      <c r="Z5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AC5" s="10" t="s">
+      <c r="AC5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AD5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE5" s="10" t="s">
+      <c r="AD5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AF5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH5" s="10" t="s">
+      <c r="AF5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AI5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AK5" s="10" t="s">
+      <c r="AI5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK5" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AL5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AN5" s="10" t="s">
+      <c r="AL5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AO5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ5" s="13" t="s">
+      <c r="AO5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ5" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AR5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS5" s="10" t="s">
+      <c r="AR5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS5" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="AT5" s="10"/>
+      <c r="AT5" s="9"/>
     </row>
-    <row r="6" s="14" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+    <row r="6" s="12" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="17" t="s">
+      <c r="C6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="E6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="8" t="s">
+      <c r="I6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M6" s="9" t="s">
+      <c r="K6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="P6" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="S6" s="10" t="s">
+      <c r="N6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="T6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="U6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="V6" s="12" t="s">
+      <c r="T6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="U6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="V6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="W6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="X6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y6" s="10" t="s">
+      <c r="W6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="X6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Z6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB6" s="10" t="s">
+      <c r="Z6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AC6" s="10" t="s">
+      <c r="AC6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AD6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE6" s="10" t="s">
+      <c r="AD6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AF6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH6" s="10" t="s">
+      <c r="AF6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AI6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AK6" s="10" t="s">
+      <c r="AI6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK6" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AL6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AN6" s="10" t="s">
+      <c r="AL6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN6" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AO6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ6" s="13" t="s">
+      <c r="AO6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP6" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ6" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AR6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS6" s="10" t="s">
+      <c r="AR6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="AT6" s="10"/>
+      <c r="AT6" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>